<commit_message>
Expanded all rooms' MTRX Macro arrays
</commit_message>
<xml_diff>
--- a/DataFiles/RELAY TABLE SCHEDULE_022719.xlsx
+++ b/DataFiles/RELAY TABLE SCHEDULE_022719.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://l3av-my.sharepoint.com/personal/gklinger_l3av_com/Documents/Desktop/HISB Lists PRoject/gk fork/ua_hsib/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bcampagnola\Documents\L3AV\Jobs\UofA HSIB\ua_hsib_simpl\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="63" documentId="8_{07145F91-4FA9-4C5D-BE65-EA55C6AA9650}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7F1ADB90-4FA5-4BDC-94DB-3C2A6D52201F}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A2DD0F-53C6-40EC-8C17-94B823B21BE7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{2C6F9340-9CFD-4093-959A-5EA21CCB840D}"/>
+    <workbookView xWindow="29520" yWindow="1905" windowWidth="26955" windowHeight="11955" xr2:uid="{2C6F9340-9CFD-4093-959A-5EA21CCB840D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="67">
   <si>
     <t>ROOM NAME</t>
   </si>
@@ -346,6 +346,21 @@
   </si>
   <si>
     <t>RELATIVE RELAY NUMBERS</t>
+  </si>
+  <si>
+    <t>PROJ SCREEN</t>
+  </si>
+  <si>
+    <t>513A (BIOCOMM RACKS)</t>
+  </si>
+  <si>
+    <t>PRO3</t>
+  </si>
+  <si>
+    <t>CP 5A-1</t>
+  </si>
+  <si>
+    <t>local</t>
   </si>
 </sst>
 </file>
@@ -735,11 +750,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5E8515-85B4-4268-92A9-CD86796E717E}">
-  <dimension ref="A1:K73"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26:G27"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F74" sqref="F74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2039,7 +2054,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="65" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F65" t="s">
         <v>46</v>
       </c>
@@ -2059,7 +2074,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="66" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
         <v>47</v>
       </c>
@@ -2070,7 +2085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
         <v>47</v>
       </c>
@@ -2081,7 +2096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
         <v>47</v>
       </c>
@@ -2092,7 +2107,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F69" t="s">
         <v>47</v>
       </c>
@@ -2103,7 +2118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F70" t="s">
         <v>47</v>
       </c>
@@ -2114,7 +2129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="71" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F71" t="s">
         <v>47</v>
       </c>
@@ -2125,7 +2140,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="72" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F72" t="s">
         <v>47</v>
       </c>
@@ -2136,7 +2151,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="73" spans="6:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
         <v>47</v>
       </c>
@@ -2145,6 +2160,55 @@
       </c>
       <c r="H73">
         <v>8</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>63</v>
+      </c>
+      <c r="B74" t="s">
+        <v>35</v>
+      </c>
+      <c r="C74" t="s">
+        <v>64</v>
+      </c>
+      <c r="D74" t="s">
+        <v>65</v>
+      </c>
+      <c r="E74" t="s">
+        <v>66</v>
+      </c>
+      <c r="G74">
+        <v>49</v>
+      </c>
+      <c r="H74">
+        <v>1</v>
+      </c>
+      <c r="I74" t="s">
+        <v>49</v>
+      </c>
+      <c r="J74" s="3">
+        <v>567</v>
+      </c>
+      <c r="K74" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G75">
+        <v>50</v>
+      </c>
+      <c r="H75">
+        <v>2</v>
+      </c>
+      <c r="I75" t="s">
+        <v>50</v>
+      </c>
+      <c r="J75" s="3">
+        <v>567</v>
+      </c>
+      <c r="K75" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2155,18 +2219,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2373,6 +2437,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63496ACB-BF86-46D8-B0A2-C7D472ED9616}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B7B9687-ABC2-43C1-8F7B-475A0E5634C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2385,14 +2457,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="101f6e2e-80ab-440b-b33c-93c4449abb9d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63496ACB-BF86-46D8-B0A2-C7D472ED9616}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>